<commit_message>
returns ending position of all balls
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="temp" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -410,11 +410,11 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -430,27 +430,27 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Kinestic</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>15:45:08.862921</t>
+          <t>15:55:31.221782</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>15:45:13.552451</t>
+          <t>15:55:35.400989</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -471,22 +471,22 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>15:45:19.240041</t>
+          <t>15:55:41.436190</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>15:45:23.914775</t>
+          <t>15:55:46.129023</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -502,27 +502,27 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Visual</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>15:45:29.775139</t>
+          <t>15:55:52.192796</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>15:45:33.894231</t>
+          <t>15:55:57.238017</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -538,27 +538,27 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Kinestic</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>15:45:39.770330</t>
+          <t>15:56:03.318454</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>15:45:43.899966</t>
+          <t>15:56:08.389773</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -574,27 +574,27 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Visual</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>15:45:49.800387</t>
+          <t>15:56:14.453446</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>15:45:54.667556</t>
+          <t>15:56:19.011669</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -615,22 +615,22 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>15:46:00.683515</t>
+          <t>15:56:25.041341</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>15:46:05.387527</t>
+          <t>15:56:30.097322</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -651,22 +651,22 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>15:46:11.472798</t>
+          <t>15:56:36.158616</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>15:46:16.180703</t>
+          <t>15:56:41.231065</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -687,22 +687,22 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>15:46:22.237572</t>
+          <t>15:56:47.278505</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>15:46:26.961903</t>
+          <t>15:56:52.314788</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -718,27 +718,27 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Visual</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>15:46:33.123412</t>
+          <t>15:56:58.399139</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>15:46:37.843305</t>
+          <t>15:57:02.960623</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -759,22 +759,22 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>15:46:43.952424</t>
+          <t>15:57:09.046768</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>15:46:48.604600</t>
+          <t>15:57:14.105278</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -790,27 +790,27 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Kinestic</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>15:46:54.596217</t>
+          <t>15:57:20.175255</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>15:46:58.836798</t>
+          <t>15:57:25.218832</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -831,22 +831,22 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>15:47:04.912768</t>
+          <t>15:57:31.364629</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>15:47:09.646224</t>
+          <t>15:57:36.443085</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -862,27 +862,27 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Kinestic</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>15:47:15.736084</t>
+          <t>15:57:42.569074</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>15:47:20.445797</t>
+          <t>15:57:47.186889</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -898,27 +898,27 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Kinestic</t>
+          <t>Visual</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>15:47:26.520250</t>
+          <t>15:57:53.338331</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>15:47:30.722757</t>
+          <t>15:57:58.000812</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -934,27 +934,27 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Visual</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>15:47:36.821095</t>
+          <t>15:58:04.156940</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>15:47:41.051148</t>
+          <t>15:58:09.286592</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -970,27 +970,27 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Visual</t>
+          <t>Kinestic</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>15:47:47.163155</t>
+          <t>15:58:15.163829</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>15:47:51.303400</t>
+          <t>15:58:19.537060</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1011,22 +1011,22 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>15:47:57.400090</t>
+          <t>15:58:25.418756</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>15:48:02.487273</t>
+          <t>15:58:30.300093</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1042,27 +1042,27 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Kinestic</t>
+          <t>Visual</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>15:48:08.582616</t>
+          <t>15:58:36.433505</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>15:48:13.022318</t>
+          <t>15:58:40.847369</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1083,22 +1083,22 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>15:48:19.144612</t>
+          <t>15:58:46.969609</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>15:48:24.369798</t>
+          <t>15:58:52.018465</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1119,22 +1119,22 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>15:48:30.477776</t>
+          <t>15:58:58.061267</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>15:48:35.164261</t>
+          <t>15:59:03.097673</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1155,22 +1155,22 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>15:48:41.212399</t>
+          <t>15:59:09.158147</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>15:48:45.413751</t>
+          <t>15:59:13.708376</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1191,22 +1191,22 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>15:48:51.486629</t>
+          <t>15:59:19.802593</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>15:48:56.218265</t>
+          <t>15:59:24.883972</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1222,27 +1222,27 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Kinestic</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>15:49:02.369887</t>
+          <t>15:59:31.008496</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>15:49:07.081229</t>
+          <t>15:59:35.685135</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1263,22 +1263,22 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>15:49:13.123220</t>
+          <t>15:59:41.746635</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>15:49:18.203426</t>
+          <t>15:59:46.815395</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1299,22 +1299,22 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>15:49:24.267064</t>
+          <t>15:59:52.899851</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>15:49:29.330508</t>
+          <t>15:59:57.966242</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1335,22 +1335,22 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>15:49:35.394365</t>
+          <t>16:00:04.066441</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>15:49:40.481631</t>
+          <t>16:00:09.217937</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1371,22 +1371,22 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>15:49:46.545166</t>
+          <t>16:00:15.121511</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>15:49:51.638021</t>
+          <t>16:00:20.051573</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1402,27 +1402,27 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Kinestic</t>
+          <t>Visual</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>15:49:57.621729</t>
+          <t>16:00:26.122375</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>15:50:02.162998</t>
+          <t>16:00:30.772550</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1438,27 +1438,27 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Visual</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>15:50:07.872946</t>
+          <t>16:00:36.881526</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>15:50:12.460959</t>
+          <t>16:00:41.979977</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>15:45:08.857934</t>
+          <t>15:55:31.215029</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1479,12 +1479,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>15:50:18.204997</t>
+          <t>16:00:47.937600</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>15:50:22.937586</t>
+          <t>16:00:53.102007</t>
         </is>
       </c>
     </row>

</xml_diff>